<commit_message>
Atjauninātas statistikas pēc pēdējiem unikoda labojumiem + ::
</commit_message>
<xml_diff>
--- a/Docs/SENIE-DSL-kodi.xlsx
+++ b/Docs/SENIE-DSL-kodi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!LaumasDoc\Git\senie\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB00376-9A89-4E29-B527-613BB94AF599}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391C5CD1-E6C0-43AD-97E1-CD7BDED2AD73}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -130,9 +130,6 @@
     <t>Piezīmes par indeksāciju</t>
   </si>
   <si>
-    <t>Apokr1689/1Mak, Apokr1689/2Mak, Apokr1689/Bar, Apokr1689/Sal, Apokr1689/Sir, Apokr1689/Tob, JT1685/1J, JT1685/1Kor, JT1685/1P, JT1685/1Tes, JT1685/1Tim, JT1685/2J, JT1685/2Kor, JT1685/2P, JT1685/2Tes, JT1685/2Tim, JT1685/3J, JT1685/Apd, JT1685/Atk, JT1685/Ebr, JT1685/Ef, JT1685/Fil, JT1685/Flm, JT1685/Gal, JT1685/Jk, JT1685/Jn, JT1685/Jud, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Rm, JT1685/Tit, Lod1775_SEAPP, Manc1643_44_LVM, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mac, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ob, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah</t>
-  </si>
-  <si>
     <t>Manc1631_LVM, Manc1643_LGL, Manc1643_Syr, Rav1767_SD, VLH1685_Sal, VLH1685_Syr</t>
   </si>
   <si>
@@ -178,24 +175,12 @@
     <t>Everita:  ja ir iespēja, tad mēs ļoti gribētu šīs Bībeles (!) piezīmes tekstu arī indeksēt, jo tas ir latviski. Adrese šādam vārdlietojumam būtu tāds pat kā Bībelei: nodaļa: pants+p , piem., kaut kāds (izgudrots piemērs) 1Sam 1:4p. Savukārt tur, kur piezīme ir ne Bībeles tekstā, to var ignorēt, jo tas ir tikai atsevišķš vārds vai skaņa, kurai turklāt grūti "pielikt" adresi (precīzu rindiņu), labākajā gadījumā tā ir tikai lappuses p: Manc1631_LVM 12p (izdomāts piemērs) -- bet tas lec ārā no pārējās šī avota adreses. Ne Bībeles tekstā šis ir mazsvarīgs.</t>
   </si>
   <si>
-    <t>Apokr1689/1Mak, Apokr1689/2Mak, Apokr1689/Asar, Apokr1689/Bar, Apokr1689/Bel, Apokr1689/GabpEst, Apokr1689/Jd, Apokr1689/Man, Apokr1689/P_Sir, Apokr1689/Prolog, Apokr1689/Sal, Apokr1689/Sir, Apokr1689/Sus, Apokr1689/Tob, JT1685/1J, JT1685/1Kor, JT1685/1P, JT1685/1Tes, JT1685/1Tim, JT1685/2J, JT1685/2Kor, JT1685/2P, JT1685/2Tes, JT1685/2Tim, JT1685/3J, JT1685/Apd, JT1685/Atk, JT1685/Ebr, JT1685/Ef, JT1685/Fil, JT1685/Flm, JT1685/Gal, JT1685/Jk, JT1685/Jn, JT1685/Jud, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Prolog_Iev, JT1685/Prolog_Sat, JT1685/Prolog_Tit, JT1685/Rm, JT1685/Tit, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mac, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ob, VD1689_94/Prolog, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah</t>
-  </si>
-  <si>
-    <t>Apokr1689/1Mak, Apokr1689/2Mak, Apokr1689/Asar, Apokr1689/Bar, Apokr1689/Bel, Apokr1689/GabpEst, Apokr1689/Jd, Apokr1689/Man, Apokr1689/P_Sir, Apokr1689/Sal, Apokr1689/Sir, Apokr1689/Sus, Apokr1689/Tob, JT1685/1J, JT1685/1Kor, JT1685/1P, JT1685/1Tes, JT1685/1Tim, JT1685/2J, JT1685/2Kor, JT1685/2P, JT1685/2Tes, JT1685/2Tim, JT1685/3J, JT1685/Apd, JT1685/Atk, JT1685/Ebr, JT1685/Ef, JT1685/Fil, JT1685/Flm, JT1685/Gal, JT1685/Jk, JT1685/Jn, JT1685/Jud, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Rm, JT1685/Tit, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mac, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ob, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah</t>
-  </si>
-  <si>
     <t>m</t>
   </si>
   <si>
-    <t>Apokr1689/1Mak, Apokr1689/2Mak, Apokr1689/Asar, Apokr1689/Bar, Apokr1689/Bel, Apokr1689/GabpEst, Apokr1689/Jd, Apokr1689/Man, Apokr1689/Sal, Apokr1689/Sir, Apokr1689/Sus, Apokr1689/Tob, JT1685/1J, JT1685/1Kor, JT1685/1P, JT1685/1Tes, JT1685/1Tim, JT1685/2J, JT1685/2Kor, JT1685/2P, JT1685/2Tes, JT1685/2Tim, JT1685/3J, JT1685/Apd, JT1685/Atk, JT1685/Ebr, JT1685/Ef, JT1685/Fil, JT1685/Flm, JT1685/Gal, JT1685/Jk, JT1685/Jn, JT1685/Jud, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Rm, JT1685/Tit, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mac, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ob, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah</t>
-  </si>
-  <si>
     <t>Kaut kādi tukšumi? Normunda indeksācijas kods paredz, ka var būt sastopams @x{} bez iekavu satura.</t>
   </si>
   <si>
-    <t>EvEp1615, Glueck1699_SBM, JT1685/Mk, Manc1643_44_LVM, Manc1643_LGL, VLH1685</t>
-  </si>
-  <si>
     <t>Sheet</t>
   </si>
   <si>
@@ -271,12 +256,6 @@
     <t>Klein1672_LPG, Manc1631_LVM, Manc1643_44_LVM, Manc1643_LGL, Manc1643_Syr, Rav1767_SD, VLH1685_Sal, VLH1685_Syr</t>
   </si>
   <si>
-    <t>AP1622, Apokr1689/1Mak, Apokr1689/2Mak, Apokr1689/Asar, Apokr1689/Bar, Apokr1689/Bel, Apokr1689/GabpEst, Apokr1689/Jd, Apokr1689/Man, Apokr1689/P_Sir, Apokr1689/Prolog, Apokr1689/Sal, Apokr1689/Sir, Apokr1689/Sus, Apokr1689/Tob, Baum1699_LVV, Baumb1795_WLWJD, Bluhm1791_MWU, Br1520_PN, Bruehn1756_DLWS, CC1585, CekFJ1790_KD, CekFV1796_NL, Depk1681_90_ms, Depk1703_TSD, Depk1704_Vortr, Dres1682_SBM, Eid1701_KB, Eid1701_RA, Elg1621_GCG, Elg1672_Cat, Elg1672_EvTA, Elg1673_CS, Elg1683_DictPLL, Ench1586, Ench1615, EvEp1587, EvEp1615, EvTA1753, Fuer1650_70_1ms, Fuer1650_70_2ms, Fuhr1690_LL, GD_1698, Gis1507_PN, Glueck1699_SBM, Gr1520_PN, Hag1790_IM, Has1550_PN, JT1685/1J, JT1685/1Kor, JT1685/1P, JT1685/1Tes, JT1685/1Tim, JT1685/2J, JT1685/2Kor, JT1685/2P, JT1685/2Tes, JT1685/2Tim, JT1685/3J, JT1685/Apd, JT1685/Atk, JT1685/Ebr, JT1685/Ef, JT1685/Fil, JT1685/Flm, JT1685/Gal, JT1685/Jk, JT1685/Jn, JT1685/Jud, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Prolog_Iev, JT1685/Prolog_Sat, JT1685/Prolog_Tit, JT1685/Rm, JT1685/Tit, Klein1672_LPG, LGL1685_K1, LGL1685_V5, LPDD1704, LS1625, Lang1685_LDL_ms, Laz1557_PN, Lod1775_SEAPP, Lod1778_WTMD, Lop1800_SDLS, MD1788, Manc1631_Cat, Manc1631_LGL, Manc1631_LVM, Manc1631_Syr, Manc1637_Sal, Manc1638_L, Manc1638_PhL, Manc1638_Run, Manc1643_44_Cat, Manc1643_44_LVM, Manc1643_LGL, Manc1643_Syr, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, Meg1593_PN, Ps1615, Rav1767_SD, Reit1675_OD, Reit1675_UeP, SKL1696_KB, SKL1696_RA, SL1684, SL1789, SLM1648, StendAJ1790_LSMP, StendAJ1793_JGW, StendGF1774_AGG, StendGF1781_JGW, StendGF1789_SL, Stobbe1796_PTK, Sulc1764_ARMST, TII1790, Tetsch1784_DKTW, Thev1575_PN, UKG1693, UKG1696, UP1587, Urban1791_LKLDD, V1771_SZA, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mac, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ob, VD1689_94/Prolog, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr, Witt1696_MMID, Witt1702_PAN, ZP1685, Zv1638_VAR, Zv1681_Kok, Zv1681_Liec_1, Zv1681_Liec_2, Zv1689_Kan, Zv1689_Salsnes, Zv1698_Lig</t>
-  </si>
-  <si>
-    <t>AP1622, CC1585, CekFJ1790_KD, CekFV1796_NL, Depk1703_TSD, Depk1704_Vortr, Dres1682_SBM, Eid1701_KB, Elg1672_Cat, Elg1672_EvTA, Elg1673_CS, Elg1683_DictPLL, Ench1586, Ench1615, EvEp1587, EvEp1615, EvTA1753, Fuhr1690_LL, GD_1698, Glueck1699_SBM, Hag1790_IM, JT1685/Prolog_Iev, Klein1672_LPG, LGL1685_K1, LGL1685_V5, LPDD1704, Lang1685_LDL_ms, Lod1775_SEAPP, Lod1778_WTMD, Lop1800_SDLS, MD1788, Manc1631_Cat, Manc1631_LGL, Manc1631_LVM, Manc1631_Syr, Manc1637_Sal, Manc1638_L, Manc1638_PhL, Manc1638_Run, Manc1643_44_Cat, Manc1643_44_LVM, Manc1643_LGL, Manc1643_Syr, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, Ps1615, Rav1767_SD, Reit1675_UeP, SKL1696_KB, SL1684, SL1789, StendAJ1790_LSMP, StendGF1774_AGG, StendGF1789_SL, Sulc1764_ARMST, TII1790, UKG1693, UKG1696, UP1587, Urban1791_LKLDD, VD1689_94/Prolog, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr</t>
-  </si>
-  <si>
     <t>Elg1621_GCG, Elg1683_DictPLL, EvTA1753, Lang1685_LDL_ms, Manc1631_LVM</t>
   </si>
   <si>
@@ -289,15 +268,6 @@
     <t>Depk1704_Vortr, Fuer1650_70_1ms, Lang1685_LDL_ms, Manc1631_Cat, Manc1631_LVM, Manc1631_Syr, Manc1643_44_Cat, Manc1643_44_LVM</t>
   </si>
   <si>
-    <t>AP1622, Apokr1689/Prolog, Apokr1689/Sal, Br1520_PN, CC1585, Depk1681_90_ms, Depk1703_TSD, Depk1704_Vortr, Dres1682_SBM, Elg1621_GCG, Elg1672_Cat, Elg1672_EvTA, Elg1673_CS, Elg1683_DictPLL, Ench1586, Ench1615, EvEp1587, EvEp1615, EvTA1753, Fuer1650_70_1ms, Fuer1650_70_2ms, GD_1698, Glueck1699_SBM, JT1685/1Kor, JT1685/1P, JT1685/2Kor, JT1685/Atk, JT1685/Jk, JT1685/Kol, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Prolog_Tit, JT1685/Rm, Klein1672_LPG, LGL1685_K1, LGL1685_V5, Lang1685_LDL_ms, Lop1800_SDLS, Manc1631_Cat, Manc1631_LGL, Manc1631_LVM, Manc1631_Syr, Manc1637_Sal, Manc1638_L, Manc1638_PhL, Manc1638_Run, Manc1643_44_Cat, Manc1643_44_LVM, Manc1643_LGL, Manc1643_Syr, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, Meg1593_PN, Ps1615, Reit1675_OD, Reit1675_UeP, SL1684, SLM1648, StendAJ1793_JGW, StendGF1774_AGG, UKG1693, UKG1696, UP1587, V1771_SZA, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/2L, VD1689_94/2Sam, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Ech, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Mac, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Prolog, VD1689_94/Ps, VD1689_94/Sak, VD1689_94/Zah, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr, Witt1702_PAN, Zv1681_Kok, Zv1681_Liec_1, Zv1689_Kan, Zv1698_Lig</t>
-  </si>
-  <si>
-    <t>AP1622, Apokr1689/2Mak, Apokr1689/Sir, Elg1673_CS, Elg1683_DictPLL, JT1685/Apd, JT1685/Ef, JT1685/Jn, JT1685/Lk, JT1685/Mk, JT1685/Mt, JT1685/Prolog_Iev, JT1685/Rm, LGL1685_V5, Manc1631_LVM, Manc1637_Sal, Manc1643_44_LVM, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, VD1689_94/1Ken, VD1689_94/1L, VD1689_94/1Moz, VD1689_94/1Sam, VD1689_94/2Ken, VD1689_94/2L, VD1689_94/2Moz, VD1689_94/2Sam, VD1689_94/3Moz, VD1689_94/4Moz, VD1689_94/5Moz, VD1689_94/Am, VD1689_94/Cef, VD1689_94/Dan, VD1689_94/Dz, VD1689_94/Ech, VD1689_94/Est, VD1689_94/Ezr, VD1689_94/Hab, VD1689_94/Hag, VD1689_94/Hoz, VD1689_94/Ij, VD1689_94/Jer, VD1689_94/Jes, VD1689_94/Jl, VD1689_94/Jon, VD1689_94/Joz, VD1689_94/Mac, VD1689_94/Mal, VD1689_94/Mih, VD1689_94/Nah, VD1689_94/Neh, VD1689_94/Ps, VD1689_94/Rdz, VD1689_94/Rut, VD1689_94/Sak, VD1689_94/Sog, VD1689_94/Zah</t>
-  </si>
-  <si>
-    <t>AP1622, Apokr1689/Prolog, Baum1699_LVV, Baumb1795_WLWJD, CC1585, Depk1681_90_ms, Depk1703_TSD, Depk1704_Vortr, Dres1682_SBM, Eid1701_KB, Eid1701_RA, Elg1621_GCG, Elg1673_CS, Ench1586, Ench1615, EvEp1587, EvEp1615, Fuer1650_70_1ms, Fuer1650_70_2ms, GD_1698, Glueck1699_SBM, Hag1790_IM, JT1685/Prolog_Iev, JT1685/Prolog_Tit, Klein1672_LPG, LGL1685_K1, LGL1685_V5, LPDD1704, LS1625, Lang1685_LDL_ms, Lod1778_WTMD, Manc1631_Cat, Manc1631_LGL, Manc1631_LVM, Manc1631_Syr, Manc1637_Sal, Manc1638_L, Manc1638_PhL, Manc1638_Run, Manc1643_44_Cat, Manc1643_44_LVM, Manc1643_LGL, Manc1643_Syr, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, Ps1615, SKL1696_KB, SL1684, StendAJ1790_LSMP, StendGF1774_AGG, StendGF1789_SL, UKG1693, UKG1696, UP1587, VD1689_94/Prolog, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr, Witt1702_PAN, Zv1638_VAR, Zv1681_Kok, Zv1681_Liec_1, Zv1681_Liec_2, Zv1689_Kan, Zv1689_Salsnes, Zv1698_Lig</t>
-  </si>
-  <si>
     <t>Nē (Normunds), Jā (Lauma)</t>
   </si>
   <si>
@@ -389,6 +359,36 @@
   </si>
   <si>
     <t>Elg1621_GCG, Manc1631_LVM, Manc1638_L, Manc1638_PhL, Manc1638_Run, StendGF1774_AGG, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr</t>
+  </si>
+  <si>
+    <t>AP1622, Apokr1689::1Mak, Apokr1689::2Mak, Apokr1689::Asar, Apokr1689::Bar, Apokr1689::Bel, Apokr1689::GabpEst, Apokr1689::Jd, Apokr1689::Man, Apokr1689::P_Sir, Apokr1689::Prolog, Apokr1689::Sal, Apokr1689::Sir, Apokr1689::Sus, Apokr1689::Tob, Baum1699_LVV, Baumb1795_WLWJD, Bluhm1791_MWU, Br1520_PN, Bruehn1756_DLWS, CC1585, CekFJ1790_KD, CekFV1796_NL, Depk1681_90_ms, Depk1703_TSD, Depk1704_Vortr, Dres1682_SBM, Eid1701_KB, Eid1701_RA, Elg1621_GCG, Elg1672_Cat, Elg1672_EvTA, Elg1673_CS, Elg1683_DictPLL, Ench1586, Ench1615, EvEp1587, EvEp1615, EvTA1753, Fuer1650_70_1ms, Fuer1650_70_2ms, Fuhr1690_LL, GD_1698, Gis1507_PN, Glueck1699_SBM, Gr1520_PN, Hag1790_IM, Has1550_PN, JT1685::1J, JT1685::1Kor, JT1685::1P, JT1685::1Tes, JT1685::1Tim, JT1685::2J, JT1685::2Kor, JT1685::2P, JT1685::2Tes, JT1685::2Tim, JT1685::3J, JT1685::Apd, JT1685::Atk, JT1685::Ebr, JT1685::Ef, JT1685::Fil, JT1685::Flm, JT1685::Gal, JT1685::Jk, JT1685::Jn, JT1685::Jud, JT1685::Kol, JT1685::Lk, JT1685::Mk, JT1685::Mt, JT1685::Prolog_Iev, JT1685::Prolog_Sat, JT1685::Prolog_Tit, JT1685::Rm, JT1685::Tit, Klein1672_LPG, LGL1685_K1, LGL1685_V5, LPDD1704, LS1625, Lang1685_LDL_ms, Laz1557_PN, Lod1775_SEAPP, Lod1778_WTMD, Lop1800_SDLS, MD1788, Manc1631_Cat, Manc1631_LGL, Manc1631_LVM, Manc1631_Syr, Manc1637_Sal, Manc1638_L, Manc1638_PhL, Manc1638_Run, Manc1643_44_Cat, Manc1643_44_LVM, Manc1643_LGL, Manc1643_Syr, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, Meg1593_PN, Ps1615, Rav1767_SD, Reit1675_OD, Reit1675_UeP, SKL1696_KB, SKL1696_RA, SL1684, SL1789, SLM1648, StendAJ1790_LSMP, StendAJ1793_JGW, StendGF1774_AGG, StendGF1781_JGW, StendGF1789_SL, Stobbe1796_PTK, Sulc1764_ARMST, TII1790, Tetsch1784_DKTW, Thev1575_PN, UKG1693, UKG1696, UP1587, Urban1791_LKLDD, V1771_SZA, VD1689_94::1Ken, VD1689_94::1L, VD1689_94::1Moz, VD1689_94::1Sam, VD1689_94::2Ken, VD1689_94::2L, VD1689_94::2Moz, VD1689_94::2Sam, VD1689_94::3Moz, VD1689_94::4Moz, VD1689_94::5Moz, VD1689_94::Am, VD1689_94::Cef, VD1689_94::Dan, VD1689_94::Dz, VD1689_94::Ech, VD1689_94::Est, VD1689_94::Ezr, VD1689_94::Hab, VD1689_94::Hag, VD1689_94::Hoz, VD1689_94::Ij, VD1689_94::Jer, VD1689_94::Jes, VD1689_94::Jl, VD1689_94::Jon, VD1689_94::Joz, VD1689_94::Mac, VD1689_94::Mal, VD1689_94::Mih, VD1689_94::Nah, VD1689_94::Neh, VD1689_94::Ob, VD1689_94::Prolog, VD1689_94::Ps, VD1689_94::Rdz, VD1689_94::Rut, VD1689_94::Sak, VD1689_94::Sog, VD1689_94::Zah, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr, Witt1696_MMID, Witt1702_PAN, ZP1685, Zv1638_VAR, Zv1681_Kok, Zv1681_Liec_1, Zv1681_Liec_2, Zv1689_Kan, Zv1689_Salsnes, Zv1698_Lig</t>
+  </si>
+  <si>
+    <t>AP1622, CC1585, CekFJ1790_KD, CekFV1796_NL, Depk1703_TSD, Depk1704_Vortr, Dres1682_SBM, Eid1701_KB, Elg1672_Cat, Elg1672_EvTA, Elg1673_CS, Elg1683_DictPLL, Ench1586, Ench1615, EvEp1587, EvEp1615, EvTA1753, Fuhr1690_LL, GD_1698, Glueck1699_SBM, Hag1790_IM, JT1685::Prolog_Iev, Klein1672_LPG, LGL1685_K1, LGL1685_V5, LPDD1704, Lang1685_LDL_ms, Lod1775_SEAPP, Lod1778_WTMD, Lop1800_SDLS, MD1788, Manc1631_Cat, Manc1631_LGL, Manc1631_LVM, Manc1631_Syr, Manc1637_Sal, Manc1638_L, Manc1638_PhL, Manc1638_Run, Manc1643_44_Cat, Manc1643_44_LVM, Manc1643_LGL, Manc1643_Syr, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, Ps1615, Rav1767_SD, Reit1675_UeP, SKL1696_KB, SL1684, SL1789, StendAJ1790_LSMP, StendGF1774_AGG, StendGF1789_SL, Sulc1764_ARMST, TII1790, UKG1693, UKG1696, UP1587, Urban1791_LKLDD, VD1689_94::Prolog, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr</t>
+  </si>
+  <si>
+    <t>Apokr1689::1Mak, Apokr1689::2Mak, Apokr1689::Asar, Apokr1689::Bar, Apokr1689::Bel, Apokr1689::GabpEst, Apokr1689::Jd, Apokr1689::Man, Apokr1689::P_Sir, Apokr1689::Prolog, Apokr1689::Sal, Apokr1689::Sir, Apokr1689::Sus, Apokr1689::Tob, JT1685::1J, JT1685::1Kor, JT1685::1P, JT1685::1Tes, JT1685::1Tim, JT1685::2J, JT1685::2Kor, JT1685::2P, JT1685::2Tes, JT1685::2Tim, JT1685::3J, JT1685::Apd, JT1685::Atk, JT1685::Ebr, JT1685::Ef, JT1685::Fil, JT1685::Flm, JT1685::Gal, JT1685::Jk, JT1685::Jn, JT1685::Jud, JT1685::Kol, JT1685::Lk, JT1685::Mk, JT1685::Mt, JT1685::Prolog_Iev, JT1685::Prolog_Sat, JT1685::Prolog_Tit, JT1685::Rm, JT1685::Tit, VD1689_94::1Ken, VD1689_94::1L, VD1689_94::1Moz, VD1689_94::1Sam, VD1689_94::2Ken, VD1689_94::2L, VD1689_94::2Moz, VD1689_94::2Sam, VD1689_94::3Moz, VD1689_94::4Moz, VD1689_94::5Moz, VD1689_94::Am, VD1689_94::Cef, VD1689_94::Dan, VD1689_94::Dz, VD1689_94::Ech, VD1689_94::Est, VD1689_94::Ezr, VD1689_94::Hab, VD1689_94::Hag, VD1689_94::Hoz, VD1689_94::Ij, VD1689_94::Jer, VD1689_94::Jes, VD1689_94::Jl, VD1689_94::Jon, VD1689_94::Joz, VD1689_94::Mac, VD1689_94::Mal, VD1689_94::Mih, VD1689_94::Nah, VD1689_94::Neh, VD1689_94::Ob, VD1689_94::Prolog, VD1689_94::Ps, VD1689_94::Rdz, VD1689_94::Rut, VD1689_94::Sak, VD1689_94::Sog, VD1689_94::Zah</t>
+  </si>
+  <si>
+    <t>Apokr1689::1Mak, Apokr1689::2Mak, Apokr1689::Asar, Apokr1689::Bar, Apokr1689::Bel, Apokr1689::GabpEst, Apokr1689::Jd, Apokr1689::Man, Apokr1689::P_Sir, Apokr1689::Sal, Apokr1689::Sir, Apokr1689::Sus, Apokr1689::Tob, JT1685::1J, JT1685::1Kor, JT1685::1P, JT1685::1Tes, JT1685::1Tim, JT1685::2J, JT1685::2Kor, JT1685::2P, JT1685::2Tes, JT1685::2Tim, JT1685::3J, JT1685::Apd, JT1685::Atk, JT1685::Ebr, JT1685::Ef, JT1685::Fil, JT1685::Flm, JT1685::Gal, JT1685::Jk, JT1685::Jn, JT1685::Jud, JT1685::Kol, JT1685::Lk, JT1685::Mk, JT1685::Mt, JT1685::Rm, JT1685::Tit, VD1689_94::1Ken, VD1689_94::1L, VD1689_94::1Moz, VD1689_94::1Sam, VD1689_94::2Ken, VD1689_94::2L, VD1689_94::2Moz, VD1689_94::2Sam, VD1689_94::3Moz, VD1689_94::4Moz, VD1689_94::5Moz, VD1689_94::Am, VD1689_94::Cef, VD1689_94::Dan, VD1689_94::Dz, VD1689_94::Ech, VD1689_94::Est, VD1689_94::Ezr, VD1689_94::Hab, VD1689_94::Hag, VD1689_94::Hoz, VD1689_94::Ij, VD1689_94::Jer, VD1689_94::Jes, VD1689_94::Jl, VD1689_94::Jon, VD1689_94::Joz, VD1689_94::Mac, VD1689_94::Mal, VD1689_94::Mih, VD1689_94::Nah, VD1689_94::Neh, VD1689_94::Ob, VD1689_94::Ps, VD1689_94::Rdz, VD1689_94::Rut, VD1689_94::Sak, VD1689_94::Sog, VD1689_94::Zah</t>
+  </si>
+  <si>
+    <t>AP1622, Apokr1689::Prolog, Apokr1689::Sal, Br1520_PN, CC1585, Depk1681_90_ms, Depk1703_TSD, Depk1704_Vortr, Dres1682_SBM, Elg1621_GCG, Elg1672_Cat, Elg1672_EvTA, Elg1673_CS, Elg1683_DictPLL, Ench1586, Ench1615, EvEp1587, EvEp1615, EvTA1753, Fuer1650_70_1ms, Fuer1650_70_2ms, GD_1698, Glueck1699_SBM, JT1685::1Kor, JT1685::1P, JT1685::2Kor, JT1685::Atk, JT1685::Jk, JT1685::Kol, JT1685::Lk, JT1685::Mk, JT1685::Mt, JT1685::Prolog_Tit, JT1685::Rm, Klein1672_LPG, LGL1685_K1, LGL1685_V5, Lang1685_LDL_ms, Lop1800_SDLS, Manc1631_Cat, Manc1631_LGL, Manc1631_LVM, Manc1631_Syr, Manc1637_Sal, Manc1638_L, Manc1638_PhL, Manc1638_Run, Manc1643_44_Cat, Manc1643_44_LVM, Manc1643_LGL, Manc1643_Syr, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, Meg1593_PN, Ps1615, Reit1675_OD, Reit1675_UeP, SL1684, SLM1648, StendAJ1793_JGW, StendGF1774_AGG, UKG1693, UKG1696, UP1587, V1771_SZA, VD1689_94::1Ken, VD1689_94::1L, VD1689_94::2L, VD1689_94::2Sam, VD1689_94::Cef, VD1689_94::Dan, VD1689_94::Ech, VD1689_94::Ezr, VD1689_94::Hab, VD1689_94::Hoz, VD1689_94::Ij, VD1689_94::Jer, VD1689_94::Jes, VD1689_94::Mac, VD1689_94::Nah, VD1689_94::Neh, VD1689_94::Prolog, VD1689_94::Ps, VD1689_94::Sak, VD1689_94::Zah, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr, Witt1702_PAN, Zv1681_Kok, Zv1681_Liec_1, Zv1689_Kan, Zv1698_Lig</t>
+  </si>
+  <si>
+    <t>Apokr1689::1Mak, Apokr1689::2Mak, Apokr1689::Asar, Apokr1689::Bar, Apokr1689::Bel, Apokr1689::GabpEst, Apokr1689::Jd, Apokr1689::Man, Apokr1689::Sal, Apokr1689::Sir, Apokr1689::Sus, Apokr1689::Tob, JT1685::1J, JT1685::1Kor, JT1685::1P, JT1685::1Tes, JT1685::1Tim, JT1685::2J, JT1685::2Kor, JT1685::2P, JT1685::2Tes, JT1685::2Tim, JT1685::3J, JT1685::Apd, JT1685::Atk, JT1685::Ebr, JT1685::Ef, JT1685::Fil, JT1685::Flm, JT1685::Gal, JT1685::Jk, JT1685::Jn, JT1685::Jud, JT1685::Kol, JT1685::Lk, JT1685::Mk, JT1685::Mt, JT1685::Rm, JT1685::Tit, VD1689_94::1Ken, VD1689_94::1L, VD1689_94::1Moz, VD1689_94::1Sam, VD1689_94::2Ken, VD1689_94::2L, VD1689_94::2Moz, VD1689_94::2Sam, VD1689_94::3Moz, VD1689_94::4Moz, VD1689_94::5Moz, VD1689_94::Am, VD1689_94::Cef, VD1689_94::Dan, VD1689_94::Dz, VD1689_94::Ech, VD1689_94::Est, VD1689_94::Ezr, VD1689_94::Hab, VD1689_94::Hag, VD1689_94::Hoz, VD1689_94::Ij, VD1689_94::Jer, VD1689_94::Jes, VD1689_94::Jl, VD1689_94::Jon, VD1689_94::Joz, VD1689_94::Mac, VD1689_94::Mal, VD1689_94::Mih, VD1689_94::Nah, VD1689_94::Neh, VD1689_94::Ob, VD1689_94::Ps, VD1689_94::Rdz, VD1689_94::Rut, VD1689_94::Sak, VD1689_94::Sog, VD1689_94::Zah</t>
+  </si>
+  <si>
+    <t>AP1622, Apokr1689::2Mak, Apokr1689::Sir, Elg1673_CS, Elg1683_DictPLL, JT1685::Apd, JT1685::Ef, JT1685::Jn, JT1685::Lk, JT1685::Mk, JT1685::Mt, JT1685::Prolog_Iev, JT1685::Rm, LGL1685_V5, Manc1631_LVM, Manc1637_Sal, Manc1643_44_LVM, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, VD1689_94::1Ken, VD1689_94::1L, VD1689_94::1Moz, VD1689_94::1Sam, VD1689_94::2Ken, VD1689_94::2L, VD1689_94::2Moz, VD1689_94::2Sam, VD1689_94::3Moz, VD1689_94::4Moz, VD1689_94::5Moz, VD1689_94::Am, VD1689_94::Cef, VD1689_94::Dan, VD1689_94::Dz, VD1689_94::Ech, VD1689_94::Est, VD1689_94::Ezr, VD1689_94::Hab, VD1689_94::Hag, VD1689_94::Hoz, VD1689_94::Ij, VD1689_94::Jer, VD1689_94::Jes, VD1689_94::Jl, VD1689_94::Jon, VD1689_94::Joz, VD1689_94::Mac, VD1689_94::Mal, VD1689_94::Mih, VD1689_94::Nah, VD1689_94::Neh, VD1689_94::Ps, VD1689_94::Rdz, VD1689_94::Rut, VD1689_94::Sak, VD1689_94::Sog, VD1689_94::Zah</t>
+  </si>
+  <si>
+    <t>EvEp1615, Glueck1699_SBM, JT1685::Mk, Manc1643_44_LVM, Manc1643_LGL, VLH1685</t>
+  </si>
+  <si>
+    <t>Apokr1689::1Mak, Apokr1689::2Mak, Apokr1689::Bar, Apokr1689::Sal, Apokr1689::Sir, Apokr1689::Tob, JT1685::1J, JT1685::1Kor, JT1685::1P, JT1685::1Tes, JT1685::1Tim, JT1685::2J, JT1685::2Kor, JT1685::2P, JT1685::2Tes, JT1685::2Tim, JT1685::3J, JT1685::Apd, JT1685::Atk, JT1685::Ebr, JT1685::Ef, JT1685::Fil, JT1685::Flm, JT1685::Gal, JT1685::Jk, JT1685::Jn, JT1685::Jud, JT1685::Kol, JT1685::Lk, JT1685::Mk, JT1685::Mt, JT1685::Rm, JT1685::Tit, Lod1775_SEAPP, Manc1643_44_LVM, VD1689_94::1Ken, VD1689_94::1L, VD1689_94::1Moz, VD1689_94::1Sam, VD1689_94::2Ken, VD1689_94::2L, VD1689_94::2Moz, VD1689_94::2Sam, VD1689_94::3Moz, VD1689_94::4Moz, VD1689_94::5Moz, VD1689_94::Am, VD1689_94::Cef, VD1689_94::Dan, VD1689_94::Dz, VD1689_94::Ech, VD1689_94::Est, VD1689_94::Ezr, VD1689_94::Hab, VD1689_94::Hag, VD1689_94::Hoz, VD1689_94::Ij, VD1689_94::Jer, VD1689_94::Jes, VD1689_94::Jl, VD1689_94::Jon, VD1689_94::Joz, VD1689_94::Mac, VD1689_94::Mal, VD1689_94::Mih, VD1689_94::Nah, VD1689_94::Neh, VD1689_94::Ob, VD1689_94::Ps, VD1689_94::Rdz, VD1689_94::Rut, VD1689_94::Sak, VD1689_94::Sog, VD1689_94::Zah</t>
+  </si>
+  <si>
+    <t>AP1622, Apokr1689::Prolog, Baum1699_LVV, Baumb1795_WLWJD, CC1585, Depk1681_90_ms, Depk1703_TSD, Depk1704_Vortr, Dres1682_SBM, Eid1701_KB, Eid1701_RA, Elg1621_GCG, Elg1673_CS, Ench1586, Ench1615, EvEp1587, EvEp1615, Fuer1650_70_1ms, Fuer1650_70_2ms, GD_1698, Glueck1699_SBM, Hag1790_IM, JT1685::Prolog_Iev, JT1685::Prolog_Tit, Klein1672_LPG, LGL1685_K1, LGL1685_V5, LPDD1704, LS1625, Lang1685_LDL_ms, Lod1778_WTMD, Manc1631_Cat, Manc1631_LGL, Manc1631_LVM, Manc1631_Syr, Manc1637_Sal, Manc1638_L, Manc1638_PhL, Manc1638_Run, Manc1643_44_Cat, Manc1643_44_LVM, Manc1643_LGL, Manc1643_Syr, Manc1654_LP1, Manc1654_LP2, Manc1654_LP3, Ps1615, SKL1696_KB, SL1684, StendAJ1790_LSMP, StendGF1774_AGG, StendGF1789_SL, UKG1693, UKG1696, UP1587, VD1689_94::Prolog, VLH1685, VLH1685_Cat, VLH1685_Sal, VLH1685_Syr, Witt1702_PAN, Zv1638_VAR, Zv1681_Kok, Zv1681_Liec_1, Zv1681_Liec_2, Zv1689_Kan, Zv1689_Salsnes, Zv1698_Lig</t>
   </si>
 </sst>
 </file>
@@ -449,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -470,13 +470,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -817,18 +822,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.26953125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="115.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="115" style="2" customWidth="1"/>
     <col min="4" max="4" width="31.26953125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="2" bestFit="1" customWidth="1"/>
@@ -839,7 +844,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>20</v>
@@ -851,13 +856,13 @@
         <v>33</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>35</v>
@@ -866,51 +871,51 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="10" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
-        <v>80</v>
+    <row r="2" spans="1:9" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="B2" s="3">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H2" s="9"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C2" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>122</v>
+      <c r="C3" s="8" t="s">
+        <v>112</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>22</v>
@@ -918,25 +923,25 @@
     </row>
     <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B4" s="3">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
-        <v>82</v>
+      <c r="C4" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>23</v>
@@ -944,25 +949,25 @@
     </row>
     <row r="5" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B5" s="3">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
-        <v>37</v>
+      <c r="C5" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>24</v>
@@ -970,381 +975,381 @@
     </row>
     <row r="6" spans="1:9" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B6" s="3">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
-        <v>81</v>
+      <c r="C6" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B7" s="3">
         <v>5</v>
       </c>
-      <c r="C7"/>
+      <c r="C7" s="8"/>
       <c r="D7" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="319" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C8" t="s">
-        <v>83</v>
+      <c r="C8" s="8" t="s">
+        <v>113</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C9" t="s">
-        <v>84</v>
+      <c r="C9" s="8" t="s">
+        <v>114</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C10" t="s">
-        <v>85</v>
+      <c r="C10" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="G10" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C11" t="s">
-        <v>86</v>
+      <c r="C11" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="G11" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C12" t="s">
-        <v>87</v>
+      <c r="C12" s="8" t="s">
+        <v>80</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="G12" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="G13" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C14" t="s">
-        <v>52</v>
+      <c r="C14" s="8" t="s">
+        <v>115</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C15" t="s">
-        <v>88</v>
+      <c r="C15" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="G15" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="8" t="s">
         <v>34</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="G16" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B17" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17"/>
+        <v>37</v>
+      </c>
+      <c r="C17" s="8"/>
       <c r="D17" s="2" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="145" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C18" t="s">
-        <v>53</v>
+      <c r="C18" s="8" t="s">
+        <v>116</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="174" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C19" t="s">
-        <v>89</v>
+      <c r="C19" s="8" t="s">
+        <v>117</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="G19" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B20" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20"/>
+        <v>51</v>
+      </c>
+      <c r="C20" s="8"/>
       <c r="D20" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="145" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C21" t="s">
-        <v>55</v>
+      <c r="C21" s="8" t="s">
+        <v>118</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B22" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C22"/>
+      <c r="C22" s="8"/>
       <c r="D22" s="2" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="145" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C23" t="s">
-        <v>90</v>
+      <c r="C23" s="8" t="s">
+        <v>119</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>28</v>
@@ -1352,171 +1357,171 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B24" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C24"/>
+        <v>90</v>
+      </c>
+      <c r="C24" s="8"/>
       <c r="D24" s="2" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C25" t="s">
-        <v>57</v>
+      <c r="C25" s="8" t="s">
+        <v>120</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="E25" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="G25" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="E26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="G26" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="145" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C27" t="s">
-        <v>36</v>
+      <c r="C27" s="8" t="s">
+        <v>121</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B28" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28"/>
+        <v>38</v>
+      </c>
+      <c r="C28" s="8"/>
       <c r="D28" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C29" t="s">
-        <v>91</v>
+      <c r="C29" s="8" t="s">
+        <v>122</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E29" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="G29" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B30" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30"/>
+        <v>39</v>
+      </c>
+      <c r="C30" s="8"/>
       <c r="D30" s="2" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B31" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31"/>
+        <v>40</v>
+      </c>
+      <c r="C31" s="8"/>
       <c r="D31" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B32" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32"/>
+        <v>41</v>
+      </c>
+      <c r="C32" s="8"/>
       <c r="D32" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="319" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C33" t="s">
-        <v>83</v>
+      <c r="C33" s="8" t="s">
+        <v>113</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>